<commit_message>
add revisi test case
</commit_message>
<xml_diff>
--- a/test_case/Test Case Register, Edit, Read.xlsx
+++ b/test_case/Test Case Register, Edit, Read.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Pribadi\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafi\UPI\GitHub\EcoSphera\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0B6756-EEA5-4971-A8B4-CC3CFB4F2770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8820492-058C-44E2-B4DA-B0CB13F6B4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Data pengguna tersimpan, redirect ke halaman pilihan login atau register</t>
-  </si>
-  <si>
-    <t>Sesuai dengan ekspektasi</t>
-  </si>
-  <si>
-    <t>Valid</t>
   </si>
   <si>
     <t>RG02</t>
@@ -156,6 +150,15 @@
   </si>
   <si>
     <t>Menampilkan data bank sampah, lalu memberikan input untuk mengedit bank sampah</t>
+  </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>KET</t>
+  </si>
+  <si>
+    <t>Note: tambah test case regis dari jaki, test case logout sama edit</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -209,11 +212,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,26 +244,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,34 +585,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB192341-7296-42B4-AB17-3F9D04AC8731}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7"/>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -601,145 +621,137 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="H3" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="E7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5"/>
@@ -748,6 +760,11 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Revisi test case register, edit, read
</commit_message>
<xml_diff>
--- a/test_case/Test Case Register, Edit, Read.xlsx
+++ b/test_case/Test Case Register, Edit, Read.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafi\UPI\GitHub\EcoSphera\test_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Pribadi\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8820492-058C-44E2-B4DA-B0CB13F6B4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F363C062-6569-4D4F-9DD3-6AC27E7D6ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case Register &amp; Logout" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case Edit" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Case Read" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -52,9 +54,6 @@
   </si>
   <si>
     <t>Register menggunakan data valid</t>
-  </si>
-  <si>
-    <t>Data pengguna tersimpan, redirect ke halaman pilihan login atau register</t>
   </si>
   <si>
     <t>RG02</t>
@@ -71,9 +70,6 @@
   </si>
   <si>
     <t>RG03</t>
-  </si>
-  <si>
-    <t>Data tidak tersimpan, redirect ke halaman pilih login atau register lalu return alert message username dan password tidak boleh kosong</t>
   </si>
   <si>
     <t>1. Jalankan program
@@ -85,10 +81,6 @@
 8. Klik enter</t>
   </si>
   <si>
-    <t>1. Username: rafi
-2. Password: rafi1</t>
-  </si>
-  <si>
     <t>Register menggunakan username kosong namun password di isi</t>
   </si>
   <si>
@@ -100,10 +92,6 @@
   </si>
   <si>
     <t>1. Username:
-2. Password: rafi2</t>
-  </si>
-  <si>
-    <t>1. Username:
 2. Password:</t>
   </si>
   <si>
@@ -111,23 +99,6 @@
   </si>
   <si>
     <t>RD01</t>
-  </si>
-  <si>
-    <t>1. Jalankan program
-2. Ketik 2
-3. Masukkan Username
-4. Klik enter
-6. Masukkan Password
-7. Klik enter
-8. Ketik 2
-9. Klik enter</t>
-  </si>
-  <si>
-    <t>1. Username: rafi212
-2. Password: rafi212</t>
-  </si>
-  <si>
-    <t>Menampilkan CRUD bank sampah</t>
   </si>
   <si>
     <t>ED01</t>
@@ -152,13 +123,286 @@
     <t>Menampilkan data bank sampah, lalu memberikan input untuk mengedit bank sampah</t>
   </si>
   <si>
-    <t>Rev</t>
-  </si>
-  <si>
-    <t>KET</t>
-  </si>
-  <si>
-    <t>Note: tambah test case regis dari jaki, test case logout sama edit</t>
+    <t>Data pengguna tersimpan, redirect ke halaman pilihan login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data tidak tersimpan, menampilkan return alert message username dan password tidak boleh kosong dan kesempatan register berkurang </t>
+  </si>
+  <si>
+    <t>Menampilkan data bank sampah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                   10. Ketik 1                                      11. Klik enter              </t>
+  </si>
+  <si>
+    <t>ED02</t>
+  </si>
+  <si>
+    <t>Menginput "q" ketika mengedit bank sampah</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                                 12. Ketik q                                      13. Klik enter</t>
+  </si>
+  <si>
+    <t>Kembali ke halaman CRUD</t>
+  </si>
+  <si>
+    <t>ED03</t>
+  </si>
+  <si>
+    <t>Menginput angka sesuai yang di tampilkan</t>
+  </si>
+  <si>
+    <t>Menampilkan output untuk mengubah data bank sampah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                                 12. Ketik 1                                      13. Klik enter        </t>
+  </si>
+  <si>
+    <t>RG04</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Klik enter
+4. Masukkan Username
+6. Klik enter                                   7. Masukkan Password               8. Klik Enter                                   9. Ketik 5                                        10. Klik Enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Username: admin              2. Password: admin                   </t>
+  </si>
+  <si>
+    <t>Kembali ke halaman login</t>
+  </si>
+  <si>
+    <t>RG05</t>
+  </si>
+  <si>
+    <t>Register menggunakan symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Jalankan program
+2. Ketik 1
+3. Klik enter
+4. Masukkan Username
+6. Klik enter                                   7. Masukkan Password               8. Klik Enter                                                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Username: @#$@@           2. Password: $@%%@                 </t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, menampilkan return alert message username dan password hanya boleh menggunakan huruf, angka dan garis bawah</t>
+  </si>
+  <si>
+    <t>1. Username: admin
+2. Password: admin</t>
+  </si>
+  <si>
+    <t>1. Username:
+2. Password: admin</t>
+  </si>
+  <si>
+    <t>ED04</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik A                                13. Klik enter</t>
+  </si>
+  <si>
+    <t>Menginput dengan menggunakan huruf (kecuali q)</t>
+  </si>
+  <si>
+    <t>Memberikan alert message "Tolong masukkan angka sesuai dengan data yang ada"</t>
+  </si>
+  <si>
+    <t>ED05</t>
+  </si>
+  <si>
+    <t>Mengubah nama bank sampah dengan symbol</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik @#$@@                  15. Klik enter</t>
+  </si>
+  <si>
+    <t>ED06</t>
+  </si>
+  <si>
+    <t>Mengubah nama pengelola dengan symbol</t>
+  </si>
+  <si>
+    <t>ED07</t>
+  </si>
+  <si>
+    <t>Mengubah lokasi bank sampah dengan symbol</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, memberikan alert message "Masukkan nama bank sampah dengan benar"</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, memberikan alert message "Masukkan nama pengelola dengan benar"</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik Asolole                  15. Klik enter                           16. Ketik %@$@</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik asolole                 15. Klik enter                           16. Ketik rehan                     17. Klik enter                           18. Ketik *&amp;$@@                   19. Klik enter</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, memberikan alert message "Masukkan lokasi dengan benar"</t>
+  </si>
+  <si>
+    <t>ED08</t>
+  </si>
+  <si>
+    <t>Mengubah nomor telepon dengan symbol</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik asolole                 15. Klik enter                           16. Ketik rehan                     17. Klik enter                           18. Ketik sukabirus                   19. Klik enter                           20. Ketik #$*@^$*!@$         21. Klik enter</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, memberikan alert message "Masukkan nomor telepon dengan benar"</t>
+  </si>
+  <si>
+    <t>ED09</t>
+  </si>
+  <si>
+    <t>Mengubah harga dengan symbol</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik asolole                 15. Klik enter                           16. Ketik rehan                     17. Klik enter                           18. Ketik sukabirus                   19. Klik enter                           20. Ketik 0812975224        21. Klik enter                           22. Ketik @$@#                      23. Klik enter</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, memberikan alert message "Masukkan harga dengan benar"</t>
+  </si>
+  <si>
+    <t>ED10</t>
+  </si>
+  <si>
+    <t>Mengubah nomor telepon dengan huruf</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik asolole                 15. Klik enter                           16. Ketik rehan                     17. Klik enter                           18. Ketik sukabirus                   19. Klik enter                           20. Ketik abcdefghij           21. Klik enter</t>
+  </si>
+  <si>
+    <t>ED11</t>
+  </si>
+  <si>
+    <t>Mengubah harga dari angka ke huruf</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Klik enter
+6. Masukkan Password
+7. Klik enter
+8. Ketik 2
+9. Klik enter                                    10. Ketik 3                                      11. Klik enter                           12. Ketik 1                                13. Klik enter                           14. Ketik asolole                 15. Klik enter                           16. Ketik rehan                     17. Klik enter                           18. Ketik sukabirus                   19. Klik enter                           20. Ketik 0812975224        21. Klik enter                           22. Ketik abcdefg                     23. Klik enter</t>
+  </si>
+  <si>
+    <t>RG06</t>
+  </si>
+  <si>
+    <t>Register menggunakan spasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Username: admin 1           2. Password: admin 1                 </t>
+  </si>
+  <si>
+    <t>RG07</t>
+  </si>
+  <si>
+    <t>Register dengan username lebih dari 256 karakter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Username: a(256x)          2. Password: admin1                 </t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, menampilkan error message username melebihi 20 karakter</t>
+  </si>
+  <si>
+    <t>RG08</t>
+  </si>
+  <si>
+    <t>Register dengan username atau password mengandung unicode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Username: user 你好          2. Password: user 你好                 </t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, menampilkan error message username atau password tidak mendukung unicode</t>
   </si>
 </sst>
 </file>
@@ -189,7 +433,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -212,22 +456,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -240,9 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,17 +489,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,34 +819,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB192341-7296-42B4-AB17-3F9D04AC8731}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="12"/>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -621,149 +855,180 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -771,4 +1036,326 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F60FD40-8156-4E70-941E-254A0D50A8C9}">
+  <dimension ref="A3:G14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E180F822-0B4F-48F6-8F31-78BB7AEFF774}">
+  <dimension ref="A3:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add pengelola features n fixing exit bug
</commit_message>
<xml_diff>
--- a/test_case/Test Case Register, Edit, Read.xlsx
+++ b/test_case/Test Case Register, Edit, Read.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Pribadi\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafi\UPI\GitHub\EcoSphera\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F363C062-6569-4D4F-9DD3-6AC27E7D6ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A912E492-1554-48AA-AD5E-5A03F54BA440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case Register &amp; Logout" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="90">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -84,13 +84,6 @@
     <t>Register menggunakan username kosong namun password di isi</t>
   </si>
   <si>
-    <t>1. Jalankan program
-2. Ketik 1
-3. Klik enter
-4. Masukkan Password
-6. Klik enter</t>
-  </si>
-  <si>
     <t>1. Username:
 2. Password:</t>
   </si>
@@ -102,9 +95,6 @@
   </si>
   <si>
     <t>ED01</t>
-  </si>
-  <si>
-    <t>Edit bank sampah</t>
   </si>
   <si>
     <t>Read bank sampah</t>
@@ -390,9 +380,6 @@
     <t xml:space="preserve">1. Username: a(256x)          2. Password: admin1                 </t>
   </si>
   <si>
-    <t>Data tidak tersimpan, menampilkan error message username melebihi 20 karakter</t>
-  </si>
-  <si>
     <t>RG08</t>
   </si>
   <si>
@@ -403,6 +390,21 @@
   </si>
   <si>
     <t>Data tidak tersimpan, menampilkan error message username atau password tidak mendukung unicode</t>
+  </si>
+  <si>
+    <t>Halaman edit bank sampah</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 1
+3. Klik enter
+4. Klik enter</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, menampilkan return alert message username hanya boleh menggunakan huruf, angka dan garis bawah</t>
+  </si>
+  <si>
+    <t>Data tidak tersimpan, menampilkan error message username melebihi 30 karakter</t>
   </si>
 </sst>
 </file>
@@ -460,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,12 +500,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,23 +817,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB192341-7296-42B4-AB17-3F9D04AC8731}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="1"/>
@@ -846,7 +842,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3"/>
@@ -855,7 +851,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -878,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -889,15 +885,15 @@
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -908,124 +904,124 @@
         <v>11</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>15</v>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="11"/>
@@ -1042,22 +1038,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F60FD40-8156-4E70-941E-254A0D50A8C9}">
   <dimension ref="A3:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1080,211 +1076,211 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="145.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>59</v>
+        <v>44</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>56</v>
+    <row r="9" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>58</v>
+    <row r="10" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="288" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="D11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="D12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:7" ht="288" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>67</v>
+        <v>44</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:7" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>71</v>
+        <v>44</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -1302,18 +1298,18 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1336,21 +1332,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="160.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5"/>

</xml_diff>